<commit_message>
update today actual work hours
</commit_message>
<xml_diff>
--- a/03.12-07.12.xlsx
+++ b/03.12-07.12.xlsx
@@ -139,7 +139,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
@@ -155,6 +155,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -445,7 +448,7 @@
   <dimension ref="B2:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F7"/>
+      <selection activeCell="J6" sqref="J6:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +542,7 @@
       <c r="C6" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="9">
         <v>6.75</v>
       </c>
       <c r="E6" s="1">
@@ -549,8 +552,12 @@
         <v>7</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="5"/>
+      <c r="I6" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="J6" s="5">
+        <v>5</v>
+      </c>
       <c r="K6" s="1"/>
       <c r="L6" s="5"/>
       <c r="M6" s="6"/>
@@ -560,13 +567,15 @@
       <c r="C7" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D7" s="8"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="1">
         <v>0.80208333333333337</v>
       </c>
       <c r="F7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <v>0.875</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="1"/>
       <c r="L7" s="5"/>

</xml_diff>

<commit_message>
Update today work hours
</commit_message>
<xml_diff>
--- a/03.12-07.12.xlsx
+++ b/03.12-07.12.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>сумма</t>
   </si>
@@ -154,10 +154,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -445,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:M7"/>
+  <dimension ref="B2:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:J7"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,26 +488,26 @@
       <c r="C3" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>6.75</v>
       </c>
       <c r="E3" s="1">
         <v>0.5</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="9">
         <v>7</v>
       </c>
-      <c r="H3" s="8"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="J3" s="8">
+      <c r="J3" s="9">
         <v>3.25</v>
       </c>
       <c r="K3" s="1">
         <v>0.69791666666666663</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="9">
         <v>3</v>
       </c>
       <c r="M3" s="6">
@@ -519,20 +519,20 @@
       <c r="C4" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="1">
         <v>0.79166666666666663</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="1">
         <v>0.83333333333333337</v>
       </c>
-      <c r="J4" s="8"/>
+      <c r="J4" s="9"/>
       <c r="K4" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="L4" s="8"/>
+      <c r="L4" s="9"/>
       <c r="M4" s="6"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
@@ -542,7 +542,7 @@
       <c r="C6" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>6.75</v>
       </c>
       <c r="E6" s="1">
@@ -558,16 +558,22 @@
       <c r="J6" s="5">
         <v>5</v>
       </c>
-      <c r="K6" s="1"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="6"/>
+      <c r="K6" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="L6" s="5">
+        <v>4.25</v>
+      </c>
+      <c r="M6" s="6">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="1">
         <v>0.82291666666666663</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="8"/>
       <c r="E7" s="1">
         <v>0.80208333333333337</v>
       </c>
@@ -577,12 +583,109 @@
         <v>0.875</v>
       </c>
       <c r="J7" s="5"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="L7" s="5"/>
       <c r="M7" s="6"/>
     </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <v>43444</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <v>43445</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <v>43446</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="2">
+        <v>43447</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="2">
+        <v>43448</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="6"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="6"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="6"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="28">
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="J11:J12"/>
     <mergeCell ref="L6:L7"/>
     <mergeCell ref="M6:M7"/>
     <mergeCell ref="B3:B4"/>

</xml_diff>

<commit_message>
Update today and tomorrow time
</commit_message>
<xml_diff>
--- a/03.12-07.12.xlsx
+++ b/03.12-07.12.xlsx
@@ -23,6 +23,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Anna Sharuntsova.EXT</author>
+  </authors>
+  <commentList>
+    <comment ref="D11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Anna Sharuntsova.EXT:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+с вычетом полутора часов на английский</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
@@ -39,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +105,19 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -444,11 +491,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,10 +665,18 @@
       <c r="B11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="9"/>
+      <c r="C11" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="D11" s="9">
+        <v>4.75</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F11" s="9">
+        <v>8</v>
+      </c>
       <c r="H11" s="9"/>
       <c r="I11" s="1"/>
       <c r="J11" s="9"/>
@@ -631,9 +686,13 @@
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="7"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1">
+        <v>0.8125</v>
+      </c>
       <c r="F12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="1"/>
@@ -646,8 +705,12 @@
       <c r="B14" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="8"/>
+      <c r="C14" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4.75</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="5"/>
       <c r="H14" s="5"/>
@@ -659,8 +722,10 @@
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="8"/>
+      <c r="C15" s="1">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D15" s="5"/>
       <c r="E15" s="1"/>
       <c r="F15" s="5"/>
       <c r="H15" s="5"/>
@@ -703,5 +768,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>